<commit_message>
mettre a jour les stories et les tests
les stories lancement du jeu et menu principale sont validée
</commit_message>
<xml_diff>
--- a/Stories-SpicyNvaders-theorlando.xlsx
+++ b/Stories-SpicyNvaders-theorlando.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROJETS\Spicy nvaders\Spicy-Nvader\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\theorlando\Documents\GitHub\Spicy-Nvader\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63DAF041-C53C-402D-84F3-467D44C3F3E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{221ADD5E-F04A-4F78-9334-79CEB87FBFB2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FC1220D0-F500-4509-AEBD-73DE32FF46A9}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
   <si>
     <t>titre</t>
   </si>
@@ -60,11 +60,6 @@
 Pour sélectionner une entrée dans un menu</t>
   </si>
   <si>
-    <t>Quand je suis sur le menu principale
-A la pression des flêches haut et bas
-Le curseur de séléction change d'entrée d'une ligne dans la direction choisie</t>
-  </si>
-  <si>
     <t>Quand le curseur sélectionne l'entrée de tout en haut
 A la pression de la flèche haut
 Il ne se passe rien</t>
@@ -82,15 +77,121 @@
   <si>
     <t>Quand le jeu n'est pas lancé sur mon pc
 Au lancement de l'éxecutable
-Le jeu se lance sur le menu principale</t>
-  </si>
-  <si>
-    <t>Quand le jeu n'est pas lancé sur mon pc
+Le curseur se trouve sur l'entrée de tout en haut</t>
+  </si>
+  <si>
+    <t>Menu option</t>
+  </si>
+  <si>
+    <t>En tant que joueur,
+Je veux accéder au menu option
+afin de pouvoir modifier la difficulté et le son du jeu</t>
+  </si>
+  <si>
+    <t>Quand je suis sur le menu principale
+A la pression des flèches haut et bas
+Le curseur de séléction change d'entrée d'une ligne dans la direction choisie</t>
+  </si>
+  <si>
+    <t>En tant que joueur,
+Je veux utiliser les flèches haut/bas
+Pour sélectionner une entrée dans le menu option</t>
+  </si>
+  <si>
+    <t>Quand je suis sur le menu option
+A la pression des flèches haut et bas
+Le curseur de séléction change d'entrée d'une ligne dans la direction choisie</t>
+  </si>
+  <si>
+    <t>Pseudo avant de jouer</t>
+  </si>
+  <si>
+    <t>En tant que joueur,
+Je veux rentrer mon pseudo avant de jouer
+Afin que mon highscore s'affiche dans le menu "HIGHSCORES"</t>
+  </si>
+  <si>
+    <t>En tant que joueur sur la page d'entrée de pseudo
+En pressant entrée le pseudo s'enregistre
+Pour savoir qui vas jouer</t>
+  </si>
+  <si>
+    <t>Lancement de la partie</t>
+  </si>
+  <si>
+    <t>En tant que joueur
+Je veux que tout les éléments du jeu s'affiche correctement
+Pour pouvoir jouer dans de bonnes condition</t>
+  </si>
+  <si>
+    <t xml:space="preserve">En tant que joueur après avoir choisi l'entrée "PLAY" sur le menu principale
+une page d'entrée de pseudo s'affichage
+Pour pouvoir rentrer mon pseudo
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">En tant que joueur au lancement de la partie
+le compteur de vie s'affiche avec toute les vies
+Pour savoir combien de vie il me reste
+</t>
+  </si>
+  <si>
+    <t>En tant que joueur au lancement de la partie
+Les murs s'affichent entierement construit
+Pour pouvoir me protéger des aliens</t>
+  </si>
+  <si>
+    <t>En tant que joueur au lancement de la partie
+Le vaisseau du joueur s'affiche 
+Pour pouvoir tirer sur les aliens</t>
+  </si>
+  <si>
+    <t>En tant que joueur au lancement de la partie
+Le compteur de score s'affiche
+pour savoir mon score en temps réel</t>
+  </si>
+  <si>
+    <t>En tant que joueur au lancement de la partie
+les aliens s'affichent
+Pour pouvoir tirer sur les aliens et qu'ils nous tirent dessus</t>
+  </si>
+  <si>
+    <t>Tir des aliens</t>
+  </si>
+  <si>
+    <t>En tant que joueur quand la partie est lancée
+Les aliens tirent vers le bas à interval irrégulier
+Pour que les aliens me tirent dessus</t>
+  </si>
+  <si>
+    <t>En tant que joueur
+Je veux que les aliens me tirent dessus
+Pour avoir un adversaire digne de ce nom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quand le jeu n'est pas lancé sur mon pc
 Au lancement de l'éxecutable
-Le curseur se trouve sur l'entrée de tout en haut</t>
-  </si>
-  <si>
-    <t>Maquette</t>
+Le jeu se lance sur le menu principale </t>
+  </si>
+  <si>
+    <t>dans le menu option avec le curseur sur l'option de difficulté sélectionnée,
+a la pression de la flèche droite
+la difficulté change (facile -&gt; moyen -&gt; difficile -&gt; godmod -&gt; facile)</t>
+  </si>
+  <si>
+    <t>dans le menu option avec le curseur sur l'option de difficulté sélectionnée,
+a la pression de la flèche gauche
+la difficulté change (facile -&gt;  godmod -&gt; difficile -&gt; moyen -&gt; facile)</t>
+  </si>
+  <si>
+    <t>En tant que joueur avec le curseur sur l'option de son sélectionnée,
+a la pression de la flèche de droite
+le son change (activé -&gt; désactivé -&gt; activé)</t>
+  </si>
+  <si>
+    <t>En tant que joueur avec le curseur sur l'option de son sélectionnée,
+a la pression de la flèche de gauche
+le son change (activé -&gt; désactivé -&gt; activé)</t>
   </si>
 </sst>
 </file>
@@ -120,7 +221,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -133,8 +234,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -155,15 +262,6 @@
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -223,7 +321,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -234,14 +332,16 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -249,12 +349,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -276,16 +373,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>514350</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>129576</xdr:rowOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>43851</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -314,7 +411,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="26946225" y="504825"/>
+          <a:off x="39309675" y="3114675"/>
           <a:ext cx="6410325" cy="3625251"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -624,10 +721,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{980F9A3D-880B-4EDA-9E11-7E060A805D83}">
-  <dimension ref="A1:N31"/>
+  <dimension ref="A1:N32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -636,10 +733,9 @@
     <col min="2" max="2" width="57" customWidth="1"/>
     <col min="3" max="3" width="59.28515625" customWidth="1"/>
     <col min="4" max="4" width="58.85546875" customWidth="1"/>
-    <col min="5" max="7" width="58.7109375" customWidth="1"/>
-    <col min="8" max="8" width="31.5703125" style="12" customWidth="1"/>
-    <col min="9" max="13" width="11.42578125" style="10"/>
-    <col min="14" max="14" width="11.42578125" style="11"/>
+    <col min="5" max="9" width="58.7109375" customWidth="1"/>
+    <col min="10" max="13" width="11.42578125" style="6"/>
+    <col min="14" max="14" width="11.42578125" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -655,34 +751,33 @@
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-      <c r="N1" s="9"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="10"/>
     </row>
     <row r="2" spans="1:14" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="11" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="4"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
     </row>
     <row r="3" spans="1:14" ht="63" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -692,75 +787,123 @@
         <v>6</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="F3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H3" s="4"/>
-    </row>
-    <row r="4" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="6"/>
-    </row>
-    <row r="5" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="6"/>
-    </row>
-    <row r="6" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+    </row>
+    <row r="5" spans="1:14" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I5" s="3"/>
+    </row>
+    <row r="6" spans="1:14" ht="102" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>34</v>
+      </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
-      <c r="G6" s="6"/>
-    </row>
-    <row r="7" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="3"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+    </row>
+    <row r="7" spans="1:14" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
-      <c r="G7" s="6"/>
-    </row>
-    <row r="8" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="6"/>
-    </row>
-    <row r="9" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+    </row>
+    <row r="8" spans="1:14" ht="63" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+    </row>
+    <row r="9" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>28</v>
+      </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
-      <c r="G9" s="6"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
     </row>
     <row r="10" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
@@ -769,7 +912,9 @@
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
-      <c r="G10" s="6"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
     </row>
     <row r="11" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
@@ -778,7 +923,9 @@
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
-      <c r="G11" s="6"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
     </row>
     <row r="12" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
@@ -787,7 +934,9 @@
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
-      <c r="G12" s="6"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
     </row>
     <row r="13" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
@@ -796,7 +945,9 @@
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
-      <c r="G13" s="6"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
     </row>
     <row r="14" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
@@ -805,7 +956,9 @@
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
-      <c r="G14" s="6"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
     </row>
     <row r="15" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
@@ -814,7 +967,9 @@
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
-      <c r="G15" s="6"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
     </row>
     <row r="16" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
@@ -823,146 +978,188 @@
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
-      <c r="G16" s="6"/>
-    </row>
-    <row r="17" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+    </row>
+    <row r="17" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
-      <c r="G17" s="6"/>
-    </row>
-    <row r="18" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+    </row>
+    <row r="18" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
-      <c r="G18" s="6"/>
-    </row>
-    <row r="19" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+    </row>
+    <row r="19" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
-      <c r="G19" s="6"/>
-    </row>
-    <row r="20" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+    </row>
+    <row r="20" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
-      <c r="G20" s="6"/>
-    </row>
-    <row r="21" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
+    </row>
+    <row r="21" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
-      <c r="G21" s="6"/>
-    </row>
-    <row r="22" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+    </row>
+    <row r="22" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
-      <c r="G22" s="6"/>
-    </row>
-    <row r="23" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+    </row>
+    <row r="23" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
-      <c r="G23" s="6"/>
-    </row>
-    <row r="24" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
+    </row>
+    <row r="24" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
-      <c r="G24" s="6"/>
-    </row>
-    <row r="25" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="5"/>
+    </row>
+    <row r="25" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
-      <c r="G25" s="6"/>
-    </row>
-    <row r="26" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
+    </row>
+    <row r="26" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
-      <c r="G26" s="6"/>
-    </row>
-    <row r="27" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="5"/>
+    </row>
+    <row r="27" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
-      <c r="G27" s="6"/>
-    </row>
-    <row r="28" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G27" s="5"/>
+      <c r="H27" s="5"/>
+      <c r="I27" s="5"/>
+    </row>
+    <row r="28" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
-      <c r="G28" s="6"/>
-    </row>
-    <row r="29" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
+      <c r="I28" s="5"/>
+    </row>
+    <row r="29" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
-      <c r="G29" s="6"/>
-    </row>
-    <row r="30" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
+      <c r="I29" s="5"/>
+    </row>
+    <row r="30" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
-      <c r="G30" s="6"/>
-    </row>
-    <row r="31" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G30" s="5"/>
+      <c r="H30" s="5"/>
+      <c r="I30" s="5"/>
+    </row>
+    <row r="31" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
-      <c r="G31" s="6"/>
+      <c r="G31" s="5"/>
+      <c r="H31" s="5"/>
+      <c r="I31" s="5"/>
+    </row>
+    <row r="32" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="2"/>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="5"/>
+      <c r="I32" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="H2:H3"/>
+  <mergeCells count="1">
     <mergeCell ref="H1:N1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
affichage du menu principale
</commit_message>
<xml_diff>
--- a/Stories-SpicyNvaders-theorlando.xlsx
+++ b/Stories-SpicyNvaders-theorlando.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\theorlando\Documents\GitHub\Spicy-Nvader\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4F1EFFA-2D06-43A3-9E65-DF4F544E5D35}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ED486E6-8575-4298-B12D-1889A3DA8901}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-10785" yWindow="1755" windowWidth="21600" windowHeight="11385" xr2:uid="{FC1220D0-F500-4509-AEBD-73DE32FF46A9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FC1220D0-F500-4509-AEBD-73DE32FF46A9}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -543,6 +543,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -551,9 +554,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -926,8 +926,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{980F9A3D-880B-4EDA-9E11-7E060A805D83}">
   <dimension ref="A1:N32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -955,16 +955,16 @@
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="4"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="10"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="11"/>
     </row>
     <row r="2" spans="1:14" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="8" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -983,7 +983,7 @@
       <c r="I2" s="5"/>
     </row>
     <row r="3" spans="1:14" ht="63" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="8" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -1006,7 +1006,7 @@
       <c r="I3" s="5"/>
     </row>
     <row r="5" spans="1:14" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="8" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -1458,15 +1458,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B4B9E7C5D694AD43BF578BC0F90B54B2" ma:contentTypeVersion="11" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="0984db86dc07217f5a46f514afe4bde0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="2355ee30-94b2-4a5a-b7d7-59ce3ea1eb14" xmlns:ns4="46b00e57-26a5-4c78-86b9-22a327b96dfd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="460f8b61d47669917f380c5230989cdf" ns3:_="" ns4:_="">
     <xsd:import namespace="2355ee30-94b2-4a5a-b7d7-59ce3ea1eb14"/>
@@ -1677,6 +1668,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1684,14 +1684,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0912D6D1-7DC0-4CFF-8ECC-C25F094057A3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{590D46E6-F198-420C-846C-2B80001D3859}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1706,6 +1698,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0912D6D1-7DC0-4CFF-8ECC-C25F094057A3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
mise en place du menu option et about
</commit_message>
<xml_diff>
--- a/Stories-SpicyNvaders-theorlando.xlsx
+++ b/Stories-SpicyNvaders-theorlando.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\theorlando\Documents\GitHub\Spicy-Nvader\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ED486E6-8575-4298-B12D-1889A3DA8901}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25F10E53-1FCA-4D91-B180-000149A8A3DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FC1220D0-F500-4509-AEBD-73DE32FF46A9}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="82">
   <si>
     <t>titre</t>
   </si>
@@ -395,6 +395,24 @@
     <t>Quand le vaisseau arrive au bord de l'écran
 Le vaisseau ne peut plus se déplacer vers le côté ou il est déjà collé au bord
 Afin que le vaisseau ne disparaisse pas de l'écran</t>
+  </si>
+  <si>
+    <t>Menu About</t>
+  </si>
+  <si>
+    <t>En tant que joueur 
+Je veux avoir des infos sur la création du jeu
+Pour comprendre les motivations du dévelopeur</t>
+  </si>
+  <si>
+    <t>Dans le menu about
+Quand je presse escape
+Le menu principale s'affiche</t>
+  </si>
+  <si>
+    <t>Dans le menu principale
+Quand je choisi le menu about
+Le menu about s'affiche</t>
   </si>
 </sst>
 </file>
@@ -927,7 +945,7 @@
   <dimension ref="A1:N32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1304,11 +1322,19 @@
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
     </row>
-    <row r="20" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="3"/>
+    <row r="20" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>80</v>
+      </c>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
       <c r="G20" s="5"/>
@@ -1458,6 +1484,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B4B9E7C5D694AD43BF578BC0F90B54B2" ma:contentTypeVersion="11" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="0984db86dc07217f5a46f514afe4bde0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="2355ee30-94b2-4a5a-b7d7-59ce3ea1eb14" xmlns:ns4="46b00e57-26a5-4c78-86b9-22a327b96dfd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="460f8b61d47669917f380c5230989cdf" ns3:_="" ns4:_="">
     <xsd:import namespace="2355ee30-94b2-4a5a-b7d7-59ce3ea1eb14"/>
@@ -1668,15 +1703,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1684,6 +1710,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0912D6D1-7DC0-4CFF-8ECC-C25F094057A3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{590D46E6-F198-420C-846C-2B80001D3859}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1698,14 +1732,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0912D6D1-7DC0-4CFF-8ECC-C25F094057A3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>